<commit_message>
DATA AND PIN MAPPING UPDATE
</commit_message>
<xml_diff>
--- a/docs/MAPPING.xlsx
+++ b/docs/MAPPING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siyxu\Documents\vamk\EmbeddedSystemProject\STM32-Battery-Management\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB441FB8-0CB8-424D-B2CE-FFF0C5D75467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFF8F1F-F0CF-4609-B589-A6E2D93F6850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25470" yWindow="2280" windowWidth="23040" windowHeight="12270" activeTab="1" xr2:uid="{31B57A6A-830A-4284-BDCB-3953C63B3770}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="19236" windowHeight="11652" activeTab="1" xr2:uid="{31B57A6A-830A-4284-BDCB-3953C63B3770}"/>
   </bookViews>
   <sheets>
     <sheet name="Modbus" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="173">
   <si>
     <t>SlaveAddress</t>
   </si>
@@ -551,9 +551,6 @@
     <t>ADC_IN1</t>
   </si>
   <si>
-    <t>MUX</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -579,6 +576,12 @@
   </si>
   <si>
     <t>D10</t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>MUX output to ADC</t>
   </si>
 </sst>
 </file>
@@ -813,10 +816,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1154,10 +1157,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1206,10 +1209,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
@@ -1848,12 +1851,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16.77734375" customWidth="1"/>
+    <col min="1" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
@@ -1864,7 +1868,7 @@
         <v>141</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>160</v>
@@ -1881,7 +1885,7 @@
         <v>116</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1895,7 +1899,7 @@
         <v>161</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1935,7 +1939,7 @@
         <v>123</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,7 +2044,9 @@
       <c r="C15" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="18" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -2052,28 +2058,30 @@
       <c r="C16" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="C18" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>166</v>
+      <c r="C19" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>